<commit_message>
clase 08 portfolio management
</commit_message>
<xml_diff>
--- a/fixed_income/Clase 07 Curvas/Ejercicio Zero.xlsx
+++ b/fixed_income/Clase 07 Curvas/Ejercicio Zero.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\Desarrollo\MEF\Catedras\Economía Financiera\economia-financiera-priv\clases\Clase 07 Curvas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\Desarrollo\MEF\Catedras\Economía Financiera\economia-financiera\fixed_income\Clase 07 Curvas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53A8B9B0-31A6-4F60-8F57-70E013CBEBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CF1F55-1915-4E7C-A882-12EAA9327EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{280B6E5B-D116-4BFC-B3CF-673B06845BA7}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>3 Años</t>
   </si>
   <si>
-    <t>5 Años</t>
-  </si>
-  <si>
     <t>7 Años</t>
   </si>
   <si>
@@ -73,14 +70,18 @@
   <si>
     <t>Tasa Zero</t>
   </si>
+  <si>
+    <t>4 Años</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -197,7 +198,7 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -207,7 +208,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
@@ -232,13 +235,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
+      <xdr:colOff>244474</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1965325" cy="345672"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -252,7 +255,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4600574" y="415924"/>
+              <a:off x="4638674" y="409574"/>
               <a:ext cx="1965325" cy="345672"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -491,7 +494,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -505,7 +508,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4600574" y="415924"/>
+              <a:off x="4638674" y="409574"/>
               <a:ext cx="1965325" cy="345672"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -533,6 +536,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="es-CL" sz="1100" i="0">
                   <a:solidFill>
@@ -600,6 +604,18 @@
                 <a:t>3,73</a:t>
               </a:r>
               <a:r>
+                <a:rPr lang="es-CL" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>" </a:t>
+              </a:r>
+              <a:r>
                 <a:rPr lang="es-CL" sz="1100" b="0" i="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
@@ -609,7 +625,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>" /(</a:t>
+                <a:t>/(</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-CL" sz="1100" b="0" i="0">
@@ -1678,16 +1694,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1702,8 +1718,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4470400" y="203200"/>
-          <a:ext cx="2063750" cy="768350"/>
+          <a:off x="4610100" y="196850"/>
+          <a:ext cx="1962150" cy="736600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1818,8 +1834,8 @@
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3006726" cy="355995"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="CuadroTexto 10">
@@ -1902,7 +1918,7 @@
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>82</m:t>
+                          <m:t>72</m:t>
                         </m:r>
                       </m:num>
                       <m:den>
@@ -2012,7 +2028,7 @@
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>82</m:t>
+                          <m:t>72</m:t>
                         </m:r>
                       </m:num>
                       <m:den>
@@ -2146,7 +2162,7 @@
                             <a:ea typeface="+mn-ea"/>
                             <a:cs typeface="+mn-cs"/>
                           </a:rPr>
-                          <m:t>82</m:t>
+                          <m:t>72</m:t>
                         </m:r>
                       </m:num>
                       <m:den>
@@ -2269,7 +2285,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="CuadroTexto 10">
@@ -2311,6 +2327,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="es-CL" sz="1100" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -2339,7 +2356,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>" 82)/(</a:t>
+                <a:t>" 72)/(</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-CL" sz="1100" b="0" i="0">
@@ -2369,7 +2386,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>82</a:t>
+                <a:t>72</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-CL" sz="1100" b="0" i="0">
@@ -2395,11 +2412,47 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>+10</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-CL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>+</a:t>
+                <a:t>"</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-CL" sz="1100" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>3,</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-CL" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>72</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-CL" sz="1100" b="0" i="0">
@@ -2411,91 +2464,7 @@
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>10</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-CL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>"</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-CL" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>3,</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-CL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>82" /(1+𝑧_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-CL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>3</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-CL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t> )^</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-CL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>3</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="es-CL" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t> </a:t>
+                <a:t>" /(1+𝑧_3 )^3 </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="es-CL" sz="1100" b="0" i="0">
@@ -2514,15 +2483,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:colOff>69850</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2537,7 +2506,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="368300" y="2425700"/>
+          <a:off x="171450" y="2432050"/>
           <a:ext cx="2946400" cy="768350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2898,39 +2867,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1448094F-ED9C-4FC2-B35F-A41D00F4B83D}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="6" max="6" width="8.36328125" customWidth="1"/>
     <col min="8" max="8" width="3.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8">
         <v>45754</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7"/>
       <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -2948,8 +2918,12 @@
         <f>+B4/100</f>
         <v>3.8599999999999995E-2</v>
       </c>
+      <c r="F4">
+        <f>+$B$7/(1+E4)^1</f>
+        <v>3.6780281147698823</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -2966,8 +2940,12 @@
         <f>(103.73/I12)^(1/2) -1</f>
         <v>3.7275786194966409E-2</v>
       </c>
+      <c r="F5">
+        <f>+$B$7/(1+E5)^2</f>
+        <v>3.5503803637511648</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2980,11 +2958,18 @@
       <c r="D6" s="1">
         <v>100</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="10">
+        <f>+F18^(1/3) -1</f>
+        <v>3.7180139948155722E-2</v>
+      </c>
+      <c r="F6">
+        <f>+$B$7/(1+E6)^3</f>
+        <v>3.4237400738517327</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>3.82</v>
@@ -2995,11 +2980,14 @@
       <c r="D7" s="1">
         <v>100</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="11">
+        <f>+J17^(1/4)-1</f>
+        <v>3.8243516523017274E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
         <v>3.97</v>
@@ -3013,9 +3001,9 @@
       <c r="E8" s="1"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
         <v>4.1500000000000004</v>
@@ -3028,9 +3016,9 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1">
         <v>4.6100000000000003</v>
@@ -3043,9 +3031,9 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1">
         <v>4.58</v>
@@ -3058,10 +3046,42 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I12">
         <f>100- (3.73/(1+(B4/100)))</f>
         <v>96.408626997881768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <f>+B6/((1+E5)^2)</f>
+        <v>3.4574384694121298</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <f>+B6/(1+E4)</f>
+        <v>3.5817446562680533</v>
+      </c>
+      <c r="J16">
+        <f>100-F4-F5-F6</f>
+        <v>89.347851447627221</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <f>100-F16-F15</f>
+        <v>92.960816874319818</v>
+      </c>
+      <c r="J17">
+        <f>+(100+C7)/J16</f>
+        <v>1.1619753392822867</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <f>+(100+C6)/F17</f>
+        <v>1.1157389047067676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>